<commit_message>
small problems part 2 July 18
</commit_message>
<xml_diff>
--- a/Lesson-5-Advanced-JavaScript-Collections/Working with Callback Functions.xlsx
+++ b/Lesson-5-Advanced-JavaScript-Collections/Working with Callback Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HAL3/Documents/Software Development/JS101-Programming-Foundations-with-JavaScript/Lesson-5-Advanced-JavaScript-Collections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E60C47B-0997-3B4B-A6D6-7A07EFD79801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7050F3F-9F67-9642-9DCA-119B2452FBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3280" yWindow="460" windowWidth="25520" windowHeight="13720" xr2:uid="{9009018D-4FC0-ED49-823C-3A38145837F6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="86">
   <si>
     <t>Action</t>
   </si>
@@ -263,6 +263,42 @@
   </si>
   <si>
     <t>Yes, returned by every callback execution</t>
+  </si>
+  <si>
+    <t>[[1, 2], [3, 4]] and [5, 6]</t>
+  </si>
+  <si>
+    <t>[1, 2] and [3, 4] and 5 and 6</t>
+  </si>
+  <si>
+    <t>number or new array</t>
+  </si>
+  <si>
+    <t>Yes, used by callback execution</t>
+  </si>
+  <si>
+    <t>(+)</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>third methd call (map)</t>
+  </si>
+  <si>
+    <t>5 and 6</t>
+  </si>
+  <si>
+    <t>[1, 2] and [3, 4]</t>
+  </si>
+  <si>
+    <t>Yes, used by inner callback execution</t>
+  </si>
+  <si>
+    <t>third callback execution</t>
+  </si>
+  <si>
+    <t>New arrays</t>
   </si>
 </sst>
 </file>
@@ -581,8 +617,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>200121</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>352521</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -921,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5685E6DB-4F2A-3749-BA84-F06C16DCE50C}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1004,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1123,7 +1159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1225,7 +1261,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1242,7 +1278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1327,7 +1363,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1344,7 +1380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1516,10 +1552,10 @@
     </row>
     <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
@@ -1534,6 +1570,103 @@
     <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>